<commit_message>
index:: by sergio giraldo @ 20230305T1543CET, gpg signed
</commit_message>
<xml_diff>
--- a/excel/dados em sheets diferentes.xlsx
+++ b/excel/dados em sheets diferentes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ing-my.sharepoint.com/personal/sergio_rodrigues_giraldo_ing_com/Documents/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GK47LX/source/office/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3198859-61DA-2040-89F0-FC7AA1994470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27F9352-C1F3-3F40-9137-16A2C8C536FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20420" xr2:uid="{54D8A9DE-7808-C24F-81AA-576E07750052}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="BBB" sheetId="3" r:id="rId3"/>
     <sheet name="CCC" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -98,7 +98,7 @@
     <t>pode usar indirect para pegar a planilha automaticamente</t>
   </si>
   <si>
-    <t>as sheets auxiliares, os valores de busca tem que estar ordenados</t>
+    <t>nas sheets auxiliares, os valores de busca tem que estar ordenados</t>
   </si>
 </sst>
 </file>
@@ -182,7 +182,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -201,30 +206,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -316,6 +298,24 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -330,16 +330,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{948D4042-A46E-9F42-A213-9241D9BEC4B6}" name="Table2" displayName="Table2" ref="A1:F5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{948D4042-A46E-9F42-A213-9241D9BEC4B6}" name="Table2" displayName="Table2" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E3D19BEF-C092-E848-86B5-EB51B787E4E3}" name="worker" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{705F150D-99AC-384E-BD83-A9CFBC6A0C8E}" name="type " dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{F835CB4A-9876-6041-83BB-E4A31A86BA12}" name="scale" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{ED4F40B5-218A-464B-9542-718A225CDFEC}" name="amount" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{9A2A54EE-0189-5040-AF42-BB35FAB5B593}" name="to pay" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{E3D19BEF-C092-E848-86B5-EB51B787E4E3}" name="worker" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{705F150D-99AC-384E-BD83-A9CFBC6A0C8E}" name="type " dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F835CB4A-9876-6041-83BB-E4A31A86BA12}" name="scale" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{ED4F40B5-218A-464B-9542-718A225CDFEC}" name="amount" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{9A2A54EE-0189-5040-AF42-BB35FAB5B593}" name="to pay" dataDxfId="1">
       <calculatedColumnFormula>VLOOKUP(Table2[[#This Row],[scale]],INDIRECT("'"&amp;B2&amp;"'!$A$1:$B$100"),2,TRUE)*Table2[[#This Row],[amount]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EDD61D68-7CD0-8945-A774-30A878907D5D}" name="expected" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{EDD61D68-7CD0-8945-A774-30A878907D5D}" name="expected" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -645,7 +645,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: excel, dot in ranges;advanced filter ::by sergio giraldo @ 20250729T1753CEST, gpg signed
</commit_message>
<xml_diff>
--- a/excel/dados em sheets diferentes.xlsx
+++ b/excel/dados em sheets diferentes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GK47LX/source/office/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27F9352-C1F3-3F40-9137-16A2C8C536FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F78830-2E6F-EA40-BA0F-F77C1C1B005D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20420" xr2:uid="{54D8A9DE-7808-C24F-81AA-576E07750052}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="34560" windowHeight="20420" xr2:uid="{54D8A9DE-7808-C24F-81AA-576E07750052}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>hour</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>nas sheets auxiliares, os valores de busca tem que estar ordenados</t>
+  </si>
+  <si>
+    <t>note que o nome da minha tab eh o nome do type (AAA, BBB, CCC)</t>
   </si>
 </sst>
 </file>
@@ -155,11 +158,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,6 +196,7 @@
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -346,9 +355,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -386,7 +395,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -492,7 +501,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -634,7 +643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -645,7 +654,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -654,7 +663,7 @@
     <col min="2" max="3" width="10.83203125" style="2"/>
     <col min="4" max="4" width="12.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="22.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="2" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -674,8 +683,11 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -781,24 +793,27 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>1.2</v>
       </c>
     </row>
@@ -812,24 +827,27 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>2</v>
       </c>
     </row>
@@ -843,24 +861,27 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>